<commit_message>
Convert text numbers, bools to native types, change process to processFile, make dst dirs
Convert: recognize booleans and numbers in text and convert them to native types

Process: the core method, process, collides with node's process object. Changed
process to processFilre.

Ensure the desitnation directory exists, making it if necessary.
</commit_message>
<xml_diff>
--- a/data/col-oriented.xlsx
+++ b/data/col-oriented.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/starver/code/makara/ExcelToJson/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/starver/code/makara/excel-as-json/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16840" yWindow="4760" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="5440" yWindow="4040" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>firstName</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>stormagedden;bob</t>
+  </si>
+  <si>
+    <t>isEmployee</t>
   </si>
 </sst>
 </file>
@@ -422,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -503,56 +506,69 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
+        <v>28</v>
+      </c>
+      <c r="B7" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="C7" t="str">
+        <f>"false"</f>
+        <v>false</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added sheet number argument to processFile
</commit_message>
<xml_diff>
--- a/data/col-oriented.xlsx
+++ b/data/col-oriented.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26207"/>
-  <workbookPr showInkAnnotation="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/starver/code/makara/excel-as-json/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27729"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5440" yWindow="4040" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>firstName</t>
   </si>
@@ -111,16 +107,53 @@
   </si>
   <si>
     <t>isEmployee</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Irwin</t>
+  </si>
+  <si>
+    <t>123 Fake Street</t>
+  </si>
+  <si>
+    <t>Rochester</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>505-505-1010</t>
+  </si>
+  <si>
+    <t>binarymax;arch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -143,13 +176,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -205,7 +242,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -240,7 +277,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -417,7 +454,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -427,18 +464,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,7 +486,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -460,7 +497,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -471,7 +508,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -482,7 +519,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -493,7 +530,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -504,7 +541,7 @@
         <v>81657</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -517,7 +554,7 @@
         <v>false</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -528,7 +565,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -539,7 +576,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -550,7 +587,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -561,7 +598,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -574,5 +611,132 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>99999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="str">
+        <f>"false"</f>
+        <v>false</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>